<commit_message>
components list fixed getting data from onelec fixed
</commit_message>
<xml_diff>
--- a/Components Statistics.xlsx
+++ b/Components Statistics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="149">
   <si>
     <t>Value</t>
   </si>
@@ -460,13 +460,19 @@
   </si>
   <si>
     <t>stm32f072rbt6</t>
+  </si>
+  <si>
+    <t>47491-0001</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -488,6 +494,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -513,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -521,6 +534,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -808,7 +823,7 @@
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1135,11 +1150,11 @@
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>6</v>
       </c>
@@ -1229,13 +1244,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="E25" s="1">
         <v>4</v>
       </c>
@@ -1295,9 +1312,13 @@
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="E29" s="1">
         <v>4</v>
       </c>

</xml_diff>